<commit_message>
Fixed Puzzle 2 tables on Culling and Elitism
</commit_message>
<xml_diff>
--- a/A2/output/puzzle2/puzzle2_4c.xlsx
+++ b/A2/output/puzzle2/puzzle2_4c.xlsx
@@ -278,6 +278,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Best</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -481,6 +484,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Worst</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -684,6 +690,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>Median</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -893,11 +902,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="441381736"/>
-        <c:axId val="441378992"/>
+        <c:axId val="211662424"/>
+        <c:axId val="211661640"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="441381736"/>
+        <c:axId val="211662424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -940,7 +949,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="441378992"/>
+        <c:crossAx val="211661640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -948,7 +957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="441378992"/>
+        <c:axId val="211661640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -999,7 +1008,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="441381736"/>
+        <c:crossAx val="211662424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1936,7 +1945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="N2" workbookViewId="0">
       <selection activeCell="AE6" sqref="AE6"/>
     </sheetView>
   </sheetViews>

</xml_diff>